<commit_message>
:heavy_plus_sign: feat: Final push. Work complete.
</commit_message>
<xml_diff>
--- a/python/scripts/metadado.xlsx
+++ b/python/scripts/metadado.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Impacta/DE04/dataops/de04_dataops/aula02/scripts/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="11_AD4D361C20488DEA4E38A0B7F41969B45ADEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A8F9203-BC21-47CF-A020-10B26CA3D996}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2985" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="2985" windowWidth="21600" windowHeight="11295"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>tabela</t>
   </si>
@@ -124,13 +118,19 @@
   </si>
   <si>
     <t>dob.date</t>
+  </si>
+  <si>
+    <t>lower_case</t>
+  </si>
+  <si>
+    <t>convert_ascii</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,14 +141,6 @@
     <font>
       <b/>
       <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -176,12 +168,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,18 +445,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:O10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,12 +465,9 @@
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="33.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,13 +489,14 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -529,8 +518,14 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -552,8 +547,14 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -575,8 +576,14 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -598,8 +605,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -621,8 +634,14 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -644,8 +663,14 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -667,8 +692,14 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -690,8 +721,14 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -713,9 +750,12 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="2"/>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>